<commit_message>
fetching ids of correct answers
</commit_message>
<xml_diff>
--- a/data/BOW_data.xlsx
+++ b/data/BOW_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L190"/>
+  <dimension ref="A1:L228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8311,6 +8311,1666 @@
         <v>44921</v>
       </c>
     </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>1804</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>مش عيب تكوني حمارة خاصة اذا ميولك قواتجية بس تكوني حمارة و مدعية! يا رب ارحم و اشفي هالطفلة البلوي على اهلها و المجتمع   إلى الرب نصلي</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>0</v>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>hate</t>
+        </is>
+      </c>
+      <c r="E191" t="n">
+        <v>190</v>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>Mockery</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr"/>
+      <c r="H191" t="n">
+        <v>0</v>
+      </c>
+      <c r="I191" t="n">
+        <v>1</v>
+      </c>
+      <c r="J191" t="n">
+        <v>1804</v>
+      </c>
+      <c r="K191" t="inlineStr"/>
+      <c r="L191" s="2" t="n">
+        <v>44921</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>1804</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>مش عيب تكوني حمارة خاصة اذا ميولك قواتجية بس تكوني حمارة و مدعية! يا رب ارحم و اشفي هالطفلة البلوي على اهلها و المجتمع   إلى الرب نصلي</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
+        <v>0</v>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>hate</t>
+        </is>
+      </c>
+      <c r="E192" t="n">
+        <v>191</v>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>Racist</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr"/>
+      <c r="H192" t="n">
+        <v>0</v>
+      </c>
+      <c r="I192" t="n">
+        <v>1</v>
+      </c>
+      <c r="J192" t="n">
+        <v>1804</v>
+      </c>
+      <c r="K192" t="inlineStr"/>
+      <c r="L192" s="2" t="n">
+        <v>44921</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>3890</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>زعلان على اسيادك ياوسخة يا لاعق الاحذية</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>0</v>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>abusive</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>192</v>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>Sexual harrasment</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr"/>
+      <c r="H193" t="n">
+        <v>0</v>
+      </c>
+      <c r="I193" t="n">
+        <v>1</v>
+      </c>
+      <c r="J193" t="n">
+        <v>3890</v>
+      </c>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>ياوسخة</t>
+        </is>
+      </c>
+      <c r="L193" s="2" t="n">
+        <v>44921</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>3890</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>زعلان على اسيادك ياوسخة يا لاعق الاحذية</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>0</v>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>abusive</t>
+        </is>
+      </c>
+      <c r="E194" t="n">
+        <v>193</v>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>Mockery</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr"/>
+      <c r="H194" t="n">
+        <v>0</v>
+      </c>
+      <c r="I194" t="n">
+        <v>1</v>
+      </c>
+      <c r="J194" t="n">
+        <v>3890</v>
+      </c>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>لاعق الاحذية</t>
+        </is>
+      </c>
+      <c r="L194" s="2" t="n">
+        <v>44921</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>1110</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">كول خرا </t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>0</v>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>abusive</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>194</v>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>Violent</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr"/>
+      <c r="H195" t="n">
+        <v>0</v>
+      </c>
+      <c r="I195" t="n">
+        <v>8</v>
+      </c>
+      <c r="J195" t="n">
+        <v>1110</v>
+      </c>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>خرا</t>
+        </is>
+      </c>
+      <c r="L195" s="2" t="n">
+        <v>44921</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>4089</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">وش فيه الكلب ابن الكلب وئام القذر قلب على قطر </t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>0</v>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>abusive</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>195</v>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>Violent</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr"/>
+      <c r="H196" t="n">
+        <v>0</v>
+      </c>
+      <c r="I196" t="n">
+        <v>8</v>
+      </c>
+      <c r="J196" t="n">
+        <v>4089</v>
+      </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>الكلب</t>
+        </is>
+      </c>
+      <c r="L196" s="2" t="n">
+        <v>44921</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>4089</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">وش فيه الكلب ابن الكلب وئام القذر قلب على قطر </t>
+        </is>
+      </c>
+      <c r="C197" t="n">
+        <v>0</v>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>abusive</t>
+        </is>
+      </c>
+      <c r="E197" t="n">
+        <v>196</v>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>Violent</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr"/>
+      <c r="H197" t="n">
+        <v>0</v>
+      </c>
+      <c r="I197" t="n">
+        <v>8</v>
+      </c>
+      <c r="J197" t="n">
+        <v>4089</v>
+      </c>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>القذر</t>
+        </is>
+      </c>
+      <c r="L197" s="2" t="n">
+        <v>44921</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>3853</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اخت قطر وخنزير قطر وكل مين بيشد ع ايد خنازير قطر </t>
+        </is>
+      </c>
+      <c r="C198" t="n">
+        <v>0</v>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>hate</t>
+        </is>
+      </c>
+      <c r="E198" t="n">
+        <v>197</v>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Racist</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr"/>
+      <c r="H198" t="n">
+        <v>0</v>
+      </c>
+      <c r="I198" t="n">
+        <v>128</v>
+      </c>
+      <c r="J198" t="n">
+        <v>3853</v>
+      </c>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>ر وخنزير</t>
+        </is>
+      </c>
+      <c r="L198" s="2" t="n">
+        <v>44921</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>2119</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">مصيرك يا وئام الى مزبلة التاريخ والايام بيننا </t>
+        </is>
+      </c>
+      <c r="C199" t="n">
+        <v>0</v>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>abusive</t>
+        </is>
+      </c>
+      <c r="E199" t="n">
+        <v>198</v>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>Religious affiliation</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr"/>
+      <c r="H199" t="n">
+        <v>0</v>
+      </c>
+      <c r="I199" t="n">
+        <v>208</v>
+      </c>
+      <c r="J199" t="n">
+        <v>2119</v>
+      </c>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>مزبلة</t>
+        </is>
+      </c>
+      <c r="L199" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>1947</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">منك عارف كيف بدك تتبهدل عم تشتري البهدله لحالك مشترى البصله بصله بعمرها ما رح تصير فريزه </t>
+        </is>
+      </c>
+      <c r="C200" t="n">
+        <v>0</v>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E200" t="n">
+        <v>199</v>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>Mockery</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>لان كلمة (تتبهدل) هي كلمة يقصد بها هنا الضحك والاستهزاء وهو وضع الشخص بصورة مضحكة بواسطة التشويه او تكبير العيوب والنواقص</t>
+        </is>
+      </c>
+      <c r="H200" t="n">
+        <v>0</v>
+      </c>
+      <c r="I200" t="n">
+        <v>233</v>
+      </c>
+      <c r="J200" t="n">
+        <v>1947</v>
+      </c>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>تتبهدل</t>
+        </is>
+      </c>
+      <c r="L200" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>2999</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>لبناني قليل الحياء يستخف بالمشاهد بس هو مع من يدفع أكثر</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>0</v>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>hate</t>
+        </is>
+      </c>
+      <c r="E201" t="n">
+        <v>200</v>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>Racist</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr"/>
+      <c r="H201" t="n">
+        <v>0</v>
+      </c>
+      <c r="I201" t="n">
+        <v>233</v>
+      </c>
+      <c r="J201" t="n">
+        <v>2999</v>
+      </c>
+      <c r="K201" t="inlineStr">
+        <is>
+          <t>لبناني</t>
+        </is>
+      </c>
+      <c r="L201" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>7472</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>عم بتخيل أشكال الأبواق الجبانة وهي تسمع ماذا يقول نصرالله عن فخامة الرئيس وعن جبران باسيل والله زعلانة عليكم</t>
+        </is>
+      </c>
+      <c r="C202" t="n">
+        <v>0</v>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E202" t="n">
+        <v>201</v>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>Religious affiliation</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr"/>
+      <c r="H202" t="n">
+        <v>0</v>
+      </c>
+      <c r="I202" t="n">
+        <v>233</v>
+      </c>
+      <c r="J202" t="n">
+        <v>7472</v>
+      </c>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>الأبواق الجبانة</t>
+        </is>
+      </c>
+      <c r="L202" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>6414</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">كم نحتاج لشرفاء أمثالك حتى يكون لهذا الوطن عز وأمان </t>
+        </is>
+      </c>
+      <c r="C203" t="n">
+        <v>0</v>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E203" t="n">
+        <v>202</v>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr"/>
+      <c r="H203" t="n">
+        <v>0</v>
+      </c>
+      <c r="I203" t="n">
+        <v>233</v>
+      </c>
+      <c r="J203" t="n">
+        <v>6414</v>
+      </c>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>شرفاء أمثالك</t>
+        </is>
+      </c>
+      <c r="L203" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>1042</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>انت بوق ايراني مجوسي رخيص سعرك كلفول السوداني</t>
+        </is>
+      </c>
+      <c r="C204" t="n">
+        <v>0</v>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>hate</t>
+        </is>
+      </c>
+      <c r="E204" t="n">
+        <v>203</v>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>Violent</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr"/>
+      <c r="H204" t="n">
+        <v>0</v>
+      </c>
+      <c r="I204" t="n">
+        <v>233</v>
+      </c>
+      <c r="J204" t="n">
+        <v>1042</v>
+      </c>
+      <c r="K204" t="inlineStr">
+        <is>
+          <t>رخيص سعرك</t>
+        </is>
+      </c>
+      <c r="L204" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>2055</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>انت كلكم تبع القوات بهايم أو في جحاش وحمير وخواريف معكم هو وعم بدافع بسلاحو عن لبنان ضد اسرائيل وضد التكفيرية وما خليتو سكين ما طعنتوا فيها ولو قادرين بالسلاح كنتو مستعدين تحاربوا اتدافعوا عن حبايبكم اسرائيل وحلفائها هلأ صار بدك يا يهاجم اسرائيل والاه حيرتو سمانا انتو القوتجية</t>
+        </is>
+      </c>
+      <c r="C205" t="n">
+        <v>0</v>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>hate</t>
+        </is>
+      </c>
+      <c r="E205" t="n">
+        <v>204</v>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>Mockery</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr"/>
+      <c r="H205" t="n">
+        <v>0</v>
+      </c>
+      <c r="I205" t="n">
+        <v>233</v>
+      </c>
+      <c r="J205" t="n">
+        <v>2055</v>
+      </c>
+      <c r="K205" t="inlineStr">
+        <is>
+          <t>بهايم أو في جحاش وحمير وخواريف</t>
+        </is>
+      </c>
+      <c r="L205" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>8907</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>حسبي الله ونعم الوكيل ربي عجل قيام الساعة ربي أعن عبادك المسلمين يا رب العالمين ملينا من  مشاهدة الضلم إلاهي أعنا و لاتعن علين ونصرنا على القوم الكافرين</t>
+        </is>
+      </c>
+      <c r="C206" t="n">
+        <v>0</v>
+      </c>
+      <c r="D206" t="inlineStr"/>
+      <c r="E206" t="n">
+        <v>205</v>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>Religious affiliation</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr"/>
+      <c r="H206" t="n">
+        <v>0</v>
+      </c>
+      <c r="I206" t="n">
+        <v>233</v>
+      </c>
+      <c r="J206" t="n">
+        <v>8907</v>
+      </c>
+      <c r="K206" t="inlineStr">
+        <is>
+          <t>ل قيام الساعة</t>
+        </is>
+      </c>
+      <c r="L206" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>1251</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">شو بدك بأسمي أحترمي حالك وأحترمي ديننا الشريف وتوقفي عن الكذب وقلب الحقائق والتغطيه على من نكث بد… </t>
+        </is>
+      </c>
+      <c r="C207" t="n">
+        <v>0</v>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E207" t="n">
+        <v>206</v>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>Violent</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr"/>
+      <c r="H207" t="n">
+        <v>0</v>
+      </c>
+      <c r="I207" t="n">
+        <v>233</v>
+      </c>
+      <c r="J207" t="n">
+        <v>1251</v>
+      </c>
+      <c r="K207" t="inlineStr">
+        <is>
+          <t>أحترمي حالك وأحترمي ديننا الشريف</t>
+        </is>
+      </c>
+      <c r="L207" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>463</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">لقد تم سحقهم أيها العزيز❤ </t>
+        </is>
+      </c>
+      <c r="C208" t="n">
+        <v>0</v>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E208" t="n">
+        <v>207</v>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>Violent</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr"/>
+      <c r="H208" t="n">
+        <v>0</v>
+      </c>
+      <c r="I208" t="n">
+        <v>233</v>
+      </c>
+      <c r="J208" t="n">
+        <v>463</v>
+      </c>
+      <c r="K208" t="inlineStr">
+        <is>
+          <t>تم سحقهم أي</t>
+        </is>
+      </c>
+      <c r="L208" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>8433</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>كول هوا يازلمة</t>
+        </is>
+      </c>
+      <c r="C209" t="n">
+        <v>0</v>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>abusive</t>
+        </is>
+      </c>
+      <c r="E209" t="n">
+        <v>208</v>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>Mockery</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr"/>
+      <c r="H209" t="n">
+        <v>0</v>
+      </c>
+      <c r="I209" t="n">
+        <v>233</v>
+      </c>
+      <c r="J209" t="n">
+        <v>8433</v>
+      </c>
+      <c r="K209" t="inlineStr">
+        <is>
+          <t>كول هوا</t>
+        </is>
+      </c>
+      <c r="L209" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>5305</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">يا عيني ملا حريدة ، جريدة الاخبار للفتنة و للكذب بتحدى جريدة الاخبار تحكي عن الفساد و السرقة في مجلس الحنوب </t>
+        </is>
+      </c>
+      <c r="C210" t="n">
+        <v>0</v>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>hate</t>
+        </is>
+      </c>
+      <c r="E210" t="n">
+        <v>209</v>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>Violent</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr"/>
+      <c r="H210" t="n">
+        <v>0</v>
+      </c>
+      <c r="I210" t="n">
+        <v>233</v>
+      </c>
+      <c r="J210" t="n">
+        <v>5305</v>
+      </c>
+      <c r="K210" t="inlineStr">
+        <is>
+          <t>الاخبار للفتنة و للكذب</t>
+        </is>
+      </c>
+      <c r="L210" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>2811</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>هذه الترجمة كاملة للمقطع تاني مرة تعلمي اصول المهنة والتحقق</t>
+        </is>
+      </c>
+      <c r="C211" t="n">
+        <v>0</v>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E211" t="n">
+        <v>210</v>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr"/>
+      <c r="H211" t="n">
+        <v>0</v>
+      </c>
+      <c r="I211" t="n">
+        <v>233</v>
+      </c>
+      <c r="J211" t="n">
+        <v>2811</v>
+      </c>
+      <c r="K211" t="inlineStr">
+        <is>
+          <t>تاني مرة تعلمي</t>
+        </is>
+      </c>
+      <c r="L211" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>1346</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>الانستا يوزر كلهم بدهم حرق</t>
+        </is>
+      </c>
+      <c r="C212" t="n">
+        <v>0</v>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>hate</t>
+        </is>
+      </c>
+      <c r="E212" t="n">
+        <v>211</v>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>Violent</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr"/>
+      <c r="H212" t="n">
+        <v>0</v>
+      </c>
+      <c r="I212" t="n">
+        <v>233</v>
+      </c>
+      <c r="J212" t="n">
+        <v>1346</v>
+      </c>
+      <c r="K212" t="inlineStr">
+        <is>
+          <t>بدهم حرق</t>
+        </is>
+      </c>
+      <c r="L212" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>6742</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>النازحين السوريين بكل وقاحة بيطلعوا يطالبوا الدولة اللبنانية</t>
+        </is>
+      </c>
+      <c r="C213" t="n">
+        <v>0</v>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>hate</t>
+        </is>
+      </c>
+      <c r="E213" t="n">
+        <v>212</v>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>Racist</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr"/>
+      <c r="H213" t="n">
+        <v>0</v>
+      </c>
+      <c r="I213" t="n">
+        <v>233</v>
+      </c>
+      <c r="J213" t="n">
+        <v>6742</v>
+      </c>
+      <c r="K213" t="inlineStr">
+        <is>
+          <t>النازحين السوريين</t>
+        </is>
+      </c>
+      <c r="L213" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>6422</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>التاريخ بيتذكر رجال لهم قراراتهم كلمتهم تبقى لأجيال وأجيال عندهم خط سياسي واحد ما بزيحوا عنه أصحاب رؤيا</t>
+        </is>
+      </c>
+      <c r="C214" t="n">
+        <v>0</v>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E214" t="n">
+        <v>214</v>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr"/>
+      <c r="H214" t="n">
+        <v>0</v>
+      </c>
+      <c r="I214" t="n">
+        <v>233</v>
+      </c>
+      <c r="J214" t="n">
+        <v>6422</v>
+      </c>
+      <c r="K214" t="inlineStr">
+        <is>
+          <t>ط سياسي</t>
+        </is>
+      </c>
+      <c r="L214" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>8223</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">سيرى الناس كيف سيزحف كل من أساء لسوريا وحلفاء سوريا للأعتذار نادمين خانعين </t>
+        </is>
+      </c>
+      <c r="C215" t="n">
+        <v>0</v>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E215" t="n">
+        <v>213</v>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>Violent</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr"/>
+      <c r="H215" t="n">
+        <v>0</v>
+      </c>
+      <c r="I215" t="n">
+        <v>233</v>
+      </c>
+      <c r="J215" t="n">
+        <v>8223</v>
+      </c>
+      <c r="K215" t="inlineStr">
+        <is>
+          <t>سيزحف</t>
+        </is>
+      </c>
+      <c r="L215" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>4589</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>ما حدا بالو بطرح اسمك نحن همنا نؤمن ع حقوق المسيحيين من خلال رئيس الحمهورية ت اذا في حال انت وصلت مع اني بشك للرئاسة</t>
+        </is>
+      </c>
+      <c r="C216" t="n">
+        <v>0</v>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E216" t="n">
+        <v>215</v>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>Religious affiliation</t>
+        </is>
+      </c>
+      <c r="G216" t="inlineStr"/>
+      <c r="H216" t="n">
+        <v>0</v>
+      </c>
+      <c r="I216" t="n">
+        <v>233</v>
+      </c>
+      <c r="J216" t="n">
+        <v>4589</v>
+      </c>
+      <c r="K216" t="inlineStr">
+        <is>
+          <t>حقوق المسيحيين</t>
+        </is>
+      </c>
+      <c r="L216" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>5091</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">يا غيني ما هيدا حليف ايران ة إيران حليفة سوريا و سوريا حليفة حزب الله وانت كلب حزب الله يعني كيف زبطت معك   </t>
+        </is>
+      </c>
+      <c r="C217" t="n">
+        <v>0</v>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>abusive</t>
+        </is>
+      </c>
+      <c r="E217" t="n">
+        <v>216</v>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>Racist</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr"/>
+      <c r="H217" t="n">
+        <v>0</v>
+      </c>
+      <c r="I217" t="n">
+        <v>233</v>
+      </c>
+      <c r="J217" t="n">
+        <v>5091</v>
+      </c>
+      <c r="K217" t="inlineStr">
+        <is>
+          <t>حليفة سوريا</t>
+        </is>
+      </c>
+      <c r="L217" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>7154</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>اصلا كل البنات جاهلات</t>
+        </is>
+      </c>
+      <c r="C218" t="n">
+        <v>0</v>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>hate</t>
+        </is>
+      </c>
+      <c r="E218" t="n">
+        <v>217</v>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>Mockery</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr"/>
+      <c r="H218" t="n">
+        <v>0</v>
+      </c>
+      <c r="I218" t="n">
+        <v>233</v>
+      </c>
+      <c r="J218" t="n">
+        <v>7154</v>
+      </c>
+      <c r="K218" t="inlineStr">
+        <is>
+          <t>اهلات</t>
+        </is>
+      </c>
+      <c r="L218" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>6011</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">كان بدري عّم يقبض حق تغريدته مبارح ضد قطر   </t>
+        </is>
+      </c>
+      <c r="C219" t="n">
+        <v>0</v>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>abusive</t>
+        </is>
+      </c>
+      <c r="E219" t="n">
+        <v>218</v>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="G219" t="inlineStr"/>
+      <c r="H219" t="n">
+        <v>0</v>
+      </c>
+      <c r="I219" t="n">
+        <v>233</v>
+      </c>
+      <c r="J219" t="n">
+        <v>6011</v>
+      </c>
+      <c r="K219" t="inlineStr">
+        <is>
+          <t>عّم يقبض حق</t>
+        </is>
+      </c>
+      <c r="L219" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>5515</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>حزب الزباله و مؤيديه من بلد الزباله تفو عليكم و على الخنزير حسن زميره</t>
+        </is>
+      </c>
+      <c r="C220" t="n">
+        <v>0</v>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>hate</t>
+        </is>
+      </c>
+      <c r="E220" t="n">
+        <v>219</v>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>Violent</t>
+        </is>
+      </c>
+      <c r="G220" t="inlineStr"/>
+      <c r="H220" t="n">
+        <v>0</v>
+      </c>
+      <c r="I220" t="n">
+        <v>233</v>
+      </c>
+      <c r="J220" t="n">
+        <v>5515</v>
+      </c>
+      <c r="K220" t="inlineStr">
+        <is>
+          <t>الزباله و مؤيديه</t>
+        </is>
+      </c>
+      <c r="L220" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>6926</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>بخصوص موقف جبران باسيل بالنسبة من العداء مع اسرائيل انه ليس خلاف ايديولوجي اين بيانكم من البحث الذي توعدتم به؟</t>
+        </is>
+      </c>
+      <c r="C221" t="n">
+        <v>0</v>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E221" t="n">
+        <v>220</v>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr"/>
+      <c r="H221" t="n">
+        <v>0</v>
+      </c>
+      <c r="I221" t="n">
+        <v>233</v>
+      </c>
+      <c r="J221" t="n">
+        <v>6926</v>
+      </c>
+      <c r="K221" t="inlineStr">
+        <is>
+          <t>موقف جبران باسيل</t>
+        </is>
+      </c>
+      <c r="L221" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>8831</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>اذا الشعب اراد الحياة فلا بد ان يستجيب القدر</t>
+        </is>
+      </c>
+      <c r="C222" t="n">
+        <v>0</v>
+      </c>
+      <c r="D222" t="inlineStr"/>
+      <c r="E222" t="n">
+        <v>221</v>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="G222" t="inlineStr"/>
+      <c r="H222" t="n">
+        <v>0</v>
+      </c>
+      <c r="I222" t="n">
+        <v>233</v>
+      </c>
+      <c r="J222" t="n">
+        <v>8831</v>
+      </c>
+      <c r="K222" t="inlineStr">
+        <is>
+          <t>يستجيب القد</t>
+        </is>
+      </c>
+      <c r="L222" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>645</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>كرمال تزيد نسبة المشاهدة ما عندكن حل غير تحكوا عن جبران باسيل</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>0</v>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E223" t="n">
+        <v>222</v>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>Mockery</t>
+        </is>
+      </c>
+      <c r="G223" t="inlineStr"/>
+      <c r="H223" t="n">
+        <v>0</v>
+      </c>
+      <c r="I223" t="n">
+        <v>233</v>
+      </c>
+      <c r="J223" t="n">
+        <v>645</v>
+      </c>
+      <c r="K223" t="inlineStr">
+        <is>
+          <t>غير تحكو</t>
+        </is>
+      </c>
+      <c r="L223" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>7019</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">صباح جميل كجمال قلوبكم </t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>0</v>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E224" t="n">
+        <v>223</v>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="G224" t="inlineStr"/>
+      <c r="H224" t="n">
+        <v>0</v>
+      </c>
+      <c r="I224" t="n">
+        <v>233</v>
+      </c>
+      <c r="J224" t="n">
+        <v>7019</v>
+      </c>
+      <c r="K224" t="inlineStr">
+        <is>
+          <t>جمال قلوبكم</t>
+        </is>
+      </c>
+      <c r="L224" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>6732</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>خرسي يا كلبه يا نوريه</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
+        <v>0</v>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>hate</t>
+        </is>
+      </c>
+      <c r="E225" t="n">
+        <v>224</v>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>Violent</t>
+        </is>
+      </c>
+      <c r="G225" t="inlineStr"/>
+      <c r="H225" t="n">
+        <v>0</v>
+      </c>
+      <c r="I225" t="n">
+        <v>233</v>
+      </c>
+      <c r="J225" t="n">
+        <v>6732</v>
+      </c>
+      <c r="K225" t="inlineStr">
+        <is>
+          <t>"خرسي يا كلبه</t>
+        </is>
+      </c>
+      <c r="L225" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>7954</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>كيف بتبهدل حالك ب تلات حركات جيب جبران باسيل وعملو وزير الخارجية ويطلع يتحفنا بأفكاره دولياً مش بس محلياً</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>0</v>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E226" t="n">
+        <v>225</v>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>Mockery</t>
+        </is>
+      </c>
+      <c r="G226" t="inlineStr"/>
+      <c r="H226" t="n">
+        <v>0</v>
+      </c>
+      <c r="I226" t="n">
+        <v>233</v>
+      </c>
+      <c r="J226" t="n">
+        <v>7954</v>
+      </c>
+      <c r="K226" t="inlineStr">
+        <is>
+          <t>بتبهدل حالك</t>
+        </is>
+      </c>
+      <c r="L226" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>6214</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">شاطر ياطرنبه هذا مايريده أعداء ادروز ونت تطبل لهم يالعميل </t>
+        </is>
+      </c>
+      <c r="C227" t="n">
+        <v>0</v>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>abusive</t>
+        </is>
+      </c>
+      <c r="E227" t="n">
+        <v>226</v>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>Mockery</t>
+        </is>
+      </c>
+      <c r="G227" t="inlineStr"/>
+      <c r="H227" t="n">
+        <v>0</v>
+      </c>
+      <c r="I227" t="n">
+        <v>233</v>
+      </c>
+      <c r="J227" t="n">
+        <v>6214</v>
+      </c>
+      <c r="K227" t="inlineStr">
+        <is>
+          <t>شاطر ياطرنبه</t>
+        </is>
+      </c>
+      <c r="L227" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>1051</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>اذا موظف فجعان رئيسو قلو بعطيك كم ساعة زيادة وسب جبران باسيل شغلتنا نقعد ندافع عن نفسنا نحنا ؟؟</t>
+        </is>
+      </c>
+      <c r="C228" t="n">
+        <v>0</v>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="E228" t="n">
+        <v>227</v>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>Violent</t>
+        </is>
+      </c>
+      <c r="G228" t="inlineStr"/>
+      <c r="H228" t="n">
+        <v>0</v>
+      </c>
+      <c r="I228" t="n">
+        <v>233</v>
+      </c>
+      <c r="J228" t="n">
+        <v>1051</v>
+      </c>
+      <c r="K228" t="inlineStr">
+        <is>
+          <t>جعان</t>
+        </is>
+      </c>
+      <c r="L228" s="2" t="n">
+        <v>44924</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>